<commit_message>
add new code of local cache
</commit_message>
<xml_diff>
--- a/doc/05.Design/sdk protocal/detials of sdk protocal.xlsx
+++ b/doc/05.Design/sdk protocal/detials of sdk protocal.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7770" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="请求协议" sheetId="1" r:id="rId1"/>
+    <sheet name="返回协议" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="78">
   <si>
     <t>字段名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -303,6 +304,38 @@
   </si>
   <si>
     <t>com.xmxedu.oaken</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ad_type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>广告类型，页面跳转，文件下载，app安装，打电话</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0-页面跳转，1-文件下载，2-app安装，3-打电话</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ad_material</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>加密后的广告物料，一般是一个组装好的html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>track</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>跟踪下的展示，点击，安装的监控地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>包含展示，点击，安装三类</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -445,7 +478,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -467,18 +500,27 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -491,10 +533,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -780,8 +819,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -796,10 +835,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
+      <c r="B1" s="8"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -839,10 +878,10 @@
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="7"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="5" t="s">
         <v>14</v>
       </c>
@@ -852,10 +891,10 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="16"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
@@ -865,11 +904,11 @@
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="10" t="s">
@@ -904,17 +943,17 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="14"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="7"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="5" t="s">
         <v>1</v>
       </c>
@@ -929,7 +968,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -949,7 +988,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A12" s="13"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
@@ -967,7 +1006,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A13" s="13"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
@@ -983,7 +1022,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A14" s="13"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
@@ -999,7 +1038,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A15" s="13"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="3" t="s">
         <v>31</v>
       </c>
@@ -1015,7 +1054,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A16" s="13"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="3" t="s">
         <v>32</v>
       </c>
@@ -1031,7 +1070,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A17" s="13"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="3" t="s">
         <v>36</v>
       </c>
@@ -1047,7 +1086,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A18" s="13"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="3" t="s">
         <v>39</v>
       </c>
@@ -1065,7 +1104,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A19" s="13"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="3" t="s">
         <v>42</v>
       </c>
@@ -1083,7 +1122,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A20" s="13"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="3" t="s">
         <v>47</v>
       </c>
@@ -1099,7 +1138,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A21" s="13"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="3" t="s">
         <v>50</v>
       </c>
@@ -1115,7 +1154,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A22" s="13"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="3" t="s">
         <v>53</v>
       </c>
@@ -1131,7 +1170,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A23" s="13"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="3" t="s">
         <v>56</v>
       </c>
@@ -1147,7 +1186,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A24" s="14"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="3" t="s">
         <v>59</v>
       </c>
@@ -1161,18 +1200,18 @@
       <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="7"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="5" t="s">
         <v>1</v>
       </c>
@@ -1238,11 +1277,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A25:F25"/>
     <mergeCell ref="A27:A29"/>
@@ -1251,9 +1285,98 @@
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A9:E9"/>
     <mergeCell ref="A11:A24"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="12.875" customWidth="1"/>
+    <col min="2" max="2" width="49.125" customWidth="1"/>
+    <col min="3" max="3" width="44.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="18"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>